<commit_message>
Se realiza analisis por arboles de desiciones
</commit_message>
<xml_diff>
--- a/presentación/Rubrica_P2_DM.xlsx
+++ b/presentación/Rubrica_P2_DM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27720"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,36 +41,6 @@
     <t>Criterios de Calidad</t>
   </si>
   <si>
-    <t>Indica % de cumplimiento</t>
-  </si>
-  <si>
-    <t>Comentarios</t>
-  </si>
-  <si>
-    <t>Orden y organización de la presentación (3%)</t>
-  </si>
-  <si>
-    <t>Introducción: descripción del conjunto de datos (5%)</t>
-  </si>
-  <si>
-    <t>Presentación de resultados (5%)</t>
-  </si>
-  <si>
-    <t>Gráficos y tablas (3%)</t>
-  </si>
-  <si>
-    <t>Referencias Bibliográficas (3%)</t>
-  </si>
-  <si>
-    <t>Ortografía (3%)</t>
-  </si>
-  <si>
-    <t>Expresión Oral (8%)</t>
-  </si>
-  <si>
-    <t>Nota</t>
-  </si>
-  <si>
     <t>Excelente
 100%</t>
   </si>
@@ -91,139 +61,31 @@
 0%</t>
   </si>
   <si>
+    <t>Indica % de cumplimiento</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>Orden y organización de la presentación (3%)</t>
+  </si>
+  <si>
+    <t>La presentación esta de una manera ordenada, clara y organizada que es fácil de leer, incorporando los 5 secciones solicitadas (Introducción, desarrollo, conclusiones, referencias, anexos)</t>
+  </si>
+  <si>
+    <t>La presentación esta de una manera ordenada y organizada que es, por lo general, fácil de leer, incorporando solo 4 de las secciones solicitadas</t>
+  </si>
+  <si>
+    <t>La presentación esta de una manera desorganizada, incorporando solo 3 de las secciones solicitadas</t>
+  </si>
+  <si>
     <t>Es difícil saber qué información se relaciona, e incorpora menos de 3 secciones solicitadas</t>
   </si>
   <si>
-    <t>La presentación esta de una manera ordenada, clara y organizada que es fácil de leer, incorporando los 5 secciones solicitadas (Introducción, desarrollo, conclusiones, referencias, anexos)</t>
-  </si>
-  <si>
-    <t>La presentación esta de una manera desorganizada, incorporando solo 3 de las secciones solicitadas</t>
-  </si>
-  <si>
     <t>La presentación tiene menos de 2 secciones solicitadas</t>
   </si>
   <si>
-    <t>Cumple con 3 de los aspectos.</t>
-  </si>
-  <si>
-    <t>Cumple con 2 de los 4 aspectos.</t>
-  </si>
-  <si>
-    <t>Cumple con 1 de los 4 aspectos.</t>
-  </si>
-  <si>
-    <t>No cumple con ninguno de los aspectos.</t>
-  </si>
-  <si>
-    <t>Demuestra claridad absoluta en todo momento de la presentación, lo que se evidencia en ideas claras, pertinentes y que aportan a la exposición del trabajo.</t>
-  </si>
-  <si>
-    <t>Demuestra claridad en la presentación, pero comente errores mínimos al tratar de expresar algunas ideas que pudieran aportan a la exposición del trabajo.</t>
-  </si>
-  <si>
-    <t>Logra que su exposición sea entendible lo suficiente como para hacer que la audiencia comprenda lo mínimo de su trabajo. No aporta con ideas al trabajo.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No es claro en su discurso, expone de manera deficiente, leyendo los contenidos en vez de comentarlos.  </t>
-  </si>
-  <si>
-    <t>Confuso en sus ideas.</t>
-  </si>
-  <si>
-    <t>Los gráficos y tablas son algo difíciles de entender, no todos están debidamente referenciados.</t>
-  </si>
-  <si>
-    <t>Los gráficos y tablas son difíciles de entender o no son usados, ni referenciados.</t>
-  </si>
-  <si>
-    <t>no presenta gráficos ni tablas</t>
-  </si>
-  <si>
-    <t>Los gráficos y tablas son claros y fáciles de entender; no todos están debidamente referenciados.</t>
-  </si>
-  <si>
-    <t>Presenta 6 conclusiones claras y resumen cada una de las subsecciones del desarrollo</t>
-  </si>
-  <si>
-    <t>Presenta entre 4 y 5 conclusiones claras y resumen cada una de las subsecciones del desarrollo</t>
-  </si>
-  <si>
-    <t>Presenta entre 4 y 3 conclusiones claras y resumen cada una de las subsecciones del desarrollo</t>
-  </si>
-  <si>
-    <t>Presenta entre 1 y 2 conclusiones claras y resumen cada una de las subsecciones del desarrollo</t>
-  </si>
-  <si>
-    <t>No presenta conclusiones o no concluye respecto a cada análisis realizado.</t>
-  </si>
-  <si>
-    <t>Se apoya en más de 6 fuentes de información correctamente presentadas con uso de norma APA.</t>
-  </si>
-  <si>
-    <t>Se apoya entre 5 y 6 fuentes de información correctamente presentadas con uso de norma APA.</t>
-  </si>
-  <si>
-    <t>Se apoya entre 3 y 4 fuentes de información correctamente presentadas con uso de norma APA.</t>
-  </si>
-  <si>
-    <t>Se apoya entre 1 y 2 fuentes de información correctamente presentadas con uso de norma APA.</t>
-  </si>
-  <si>
-    <t>No especifica fuente bibliográfica de apoyo.</t>
-  </si>
-  <si>
-    <t>No tiene errores ortográficos.</t>
-  </si>
-  <si>
-    <t>Se permiten un máximo de 3 errores ortográficos.</t>
-  </si>
-  <si>
-    <t>Entre 3-8 errores ortográficos.</t>
-  </si>
-  <si>
-    <t>Más de 8-13 errores ortográficos.</t>
-  </si>
-  <si>
-    <t>Más de 13 errores ortográficos.</t>
-  </si>
-  <si>
-    <t>Utiliza vocabulario técnico y/o especializado en todo momento de la presentación.  Provee de un glosario que hace entender a la audiencia no especializada aquellos conceptos que utiliza.</t>
-  </si>
-  <si>
-    <t>Utiliza vocabulario técnico y/o especializado en la mayor parte de la presentación.  Provee de un glosario que hace entender a la audiencia no especializada aquellos conceptos que utiliza.</t>
-  </si>
-  <si>
-    <t>Utiliza vocabulario técnico y/o especializado sólo en algunos momentos de la presentación. No provee de un glosario que haga entender a la audiencia no especializada aquellos conceptos que utiliza.</t>
-  </si>
-  <si>
-    <t>El uso de vocabulario técnico es deficiente.</t>
-  </si>
-  <si>
-    <t>No utiliza vocabulario técnico en la presentación.</t>
-  </si>
-  <si>
-    <t>La presentación esta de una manera ordenada y organizada que es, por lo general, fácil de leer, incorporando solo 4 de las secciones solicitadas</t>
-  </si>
-  <si>
-    <t>Comparar el desempeño de varios algoritmos según el tipo de variable de respuesta con los datos de entrenamiento	 (20%)</t>
-  </si>
-  <si>
-    <t>Comparar el desempeño de varios algoritmos según el tipo de variable de respuesta con los datos de test e identificar cuál es el mejor algoritmo (20%)</t>
-  </si>
-  <si>
-    <t>Adjunta código utilizado
-El código es ordenado
-El código es debidamente comentado
-No presenta errores de ejecución.</t>
-  </si>
-  <si>
-    <t>Anexos (15%)</t>
-  </si>
-  <si>
-    <t>Conclusiones (15%)</t>
-  </si>
-  <si>
-    <t>Los gráficos y tablas son claros y ayudan a entender los datos, además de estar correctamente referenciados. (Árbol de desición y redes neuronales)</t>
+    <t>Introducción: descripción del conjunto de datos (5%)</t>
   </si>
   <si>
     <t>Aspectos que debe cumplir:
@@ -233,6 +95,21 @@
 -Objetivos específicos</t>
   </si>
   <si>
+    <t>Cumple con 3 de los aspectos.</t>
+  </si>
+  <si>
+    <t>Cumple con 2 de los 4 aspectos.</t>
+  </si>
+  <si>
+    <t>Cumple con 1 de los 4 aspectos.</t>
+  </si>
+  <si>
+    <t>No cumple con ninguno de los aspectos.</t>
+  </si>
+  <si>
+    <t>Comparar el desempeño de varios algoritmos según el tipo de variable de respuesta con los datos de entrenamiento	 (20%)</t>
+  </si>
+  <si>
     <t>Aspectos que debe cumplir:
 -Identifica bien el tipo de problema a resolver (regresión o clasificación) según su conjunto de datos.
 -Entrena diferentes modelos a través de la validación cruzada
@@ -240,18 +117,141 @@
 -Obtiene métricas e interpreta resultados</t>
   </si>
   <si>
+    <t>Comparar el desempeño de varios algoritmos según el tipo de variable de respuesta con los datos de test e identificar cuál es el mejor algoritmo (20%)</t>
+  </si>
+  <si>
     <t>Aspectos que debe cumplir:
 -Obtiene predicciones a través del conjunto de test 
 -Obtiene métricas con el conjunto de test.
 -Presenta los resultados y graficas.
 -Toman correcta decisión del mejor algoritmo.</t>
   </si>
+  <si>
+    <t>Presentación de resultados (5%)</t>
+  </si>
+  <si>
+    <t>Demuestra claridad absoluta en todo momento de la presentación, lo que se evidencia en ideas claras, pertinentes y que aportan a la exposición del trabajo.</t>
+  </si>
+  <si>
+    <t>Demuestra claridad en la presentación, pero comente errores mínimos al tratar de expresar algunas ideas que pudieran aportan a la exposición del trabajo.</t>
+  </si>
+  <si>
+    <t>Logra que su exposición sea entendible lo suficiente como para hacer que la audiencia comprenda lo mínimo de su trabajo. No aporta con ideas al trabajo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No es claro en su discurso, expone de manera deficiente, leyendo los contenidos en vez de comentarlos.  </t>
+  </si>
+  <si>
+    <t>Confuso en sus ideas.</t>
+  </si>
+  <si>
+    <t>Gráficos y tablas (3%)</t>
+  </si>
+  <si>
+    <t>Los gráficos y tablas son claros y ayudan a entender los datos, además de estar correctamente referenciados. (Árbol de desición y redes neuronales)</t>
+  </si>
+  <si>
+    <t>Los gráficos y tablas son claros y fáciles de entender; no todos están debidamente referenciados.</t>
+  </si>
+  <si>
+    <t>Los gráficos y tablas son algo difíciles de entender, no todos están debidamente referenciados.</t>
+  </si>
+  <si>
+    <t>Los gráficos y tablas son difíciles de entender o no son usados, ni referenciados.</t>
+  </si>
+  <si>
+    <t>no presenta gráficos ni tablas</t>
+  </si>
+  <si>
+    <t>Conclusiones (15%)</t>
+  </si>
+  <si>
+    <t>Presenta 6 conclusiones claras y resumen cada una de las subsecciones del desarrollo</t>
+  </si>
+  <si>
+    <t>Presenta entre 4 y 5 conclusiones claras y resumen cada una de las subsecciones del desarrollo</t>
+  </si>
+  <si>
+    <t>Presenta entre 4 y 3 conclusiones claras y resumen cada una de las subsecciones del desarrollo</t>
+  </si>
+  <si>
+    <t>Presenta entre 1 y 2 conclusiones claras y resumen cada una de las subsecciones del desarrollo</t>
+  </si>
+  <si>
+    <t>No presenta conclusiones o no concluye respecto a cada análisis realizado.</t>
+  </si>
+  <si>
+    <t>Referencias Bibliográficas (3%)</t>
+  </si>
+  <si>
+    <t>Se apoya en más de 6 fuentes de información correctamente presentadas con uso de norma APA.</t>
+  </si>
+  <si>
+    <t>Se apoya entre 5 y 6 fuentes de información correctamente presentadas con uso de norma APA.</t>
+  </si>
+  <si>
+    <t>Se apoya entre 3 y 4 fuentes de información correctamente presentadas con uso de norma APA.</t>
+  </si>
+  <si>
+    <t>Se apoya entre 1 y 2 fuentes de información correctamente presentadas con uso de norma APA.</t>
+  </si>
+  <si>
+    <t>No especifica fuente bibliográfica de apoyo.</t>
+  </si>
+  <si>
+    <t>Ortografía (3%)</t>
+  </si>
+  <si>
+    <t>No tiene errores ortográficos.</t>
+  </si>
+  <si>
+    <t>Se permiten un máximo de 3 errores ortográficos.</t>
+  </si>
+  <si>
+    <t>Entre 3-8 errores ortográficos.</t>
+  </si>
+  <si>
+    <t>Más de 8-13 errores ortográficos.</t>
+  </si>
+  <si>
+    <t>Más de 13 errores ortográficos.</t>
+  </si>
+  <si>
+    <t>Anexos (15%)</t>
+  </si>
+  <si>
+    <t>Adjunta código utilizado
+El código es ordenado
+El código es debidamente comentado
+No presenta errores de ejecución.</t>
+  </si>
+  <si>
+    <t>Expresión Oral (8%)</t>
+  </si>
+  <si>
+    <t>Utiliza vocabulario técnico y/o especializado en todo momento de la presentación.  Provee de un glosario que hace entender a la audiencia no especializada aquellos conceptos que utiliza.</t>
+  </si>
+  <si>
+    <t>Utiliza vocabulario técnico y/o especializado en la mayor parte de la presentación.  Provee de un glosario que hace entender a la audiencia no especializada aquellos conceptos que utiliza.</t>
+  </si>
+  <si>
+    <t>Utiliza vocabulario técnico y/o especializado sólo en algunos momentos de la presentación. No provee de un glosario que haga entender a la audiencia no especializada aquellos conceptos que utiliza.</t>
+  </si>
+  <si>
+    <t>El uso de vocabulario técnico es deficiente.</t>
+  </si>
+  <si>
+    <t>No utiliza vocabulario técnico en la presentación.</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,7 +520,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -536,7 +536,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -836,63 +836,63 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="52.88671875" customWidth="1"/>
-    <col min="2" max="2" width="64.77734375" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="26.77734375" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.21875" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="50.88671875" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" customWidth="1"/>
+    <col min="2" max="2" width="64.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H1" s="25"/>
       <c r="I1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="81.599999999999994" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G2" s="4">
         <v>1</v>
@@ -904,24 +904,24 @@
       <c r="I2" s="6"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:10" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="142.15" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G3" s="4">
         <v>1</v>
@@ -933,24 +933,24 @@
       <c r="I3" s="6"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="86.45">
       <c r="A4" s="7" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G4" s="4">
         <v>1</v>
@@ -962,24 +962,24 @@
       <c r="I4" s="6"/>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="75" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
@@ -991,24 +991,24 @@
       <c r="I5" s="6"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="95.45" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" s="4">
         <v>1</v>
@@ -1020,24 +1020,24 @@
       <c r="I6" s="6"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="86.45" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G7" s="4">
         <v>1</v>
@@ -1049,24 +1049,24 @@
       <c r="I7" s="6"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="72">
       <c r="A8" s="3" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G8" s="4">
         <v>1</v>
@@ -1078,24 +1078,24 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="72">
       <c r="A9" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G9" s="4">
         <v>1</v>
@@ -1107,24 +1107,24 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="28.9">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="G10" s="4">
         <v>1</v>
@@ -1136,24 +1136,24 @@
       <c r="I10" s="8"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="57.6">
       <c r="A11" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F11" s="22" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G11" s="4">
         <v>1</v>
@@ -1165,24 +1165,24 @@
       <c r="I11" s="8"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="100.9">
       <c r="A12" s="9" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="G12" s="4">
         <v>1</v>
@@ -1193,7 +1193,7 @@
       </c>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -1205,9 +1205,9 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="G14" s="13" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="H14" s="14">
         <f>(((H13*100)*60)/100)+10</f>

</xml_diff>

<commit_message>
Nuevas imagenes y avanace en la ppt, se crea codigo unificado para entregar a profesor
</commit_message>
<xml_diff>
--- a/presentación/Rubrica_P2_DM.xlsx
+++ b/presentación/Rubrica_P2_DM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex9\Desktop\Mineria 2023\NRC 10306\EV2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uandresbelloedu-my.sharepoint.com/personal/i_gamboaalvarado_uandresbello_edu/Documents/Documents/003_tercerAño_2024/05_mineriaDeDatos/Grupo_9/presentación/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D7FCA1-D9DB-43F3-ACEF-0B3E5FA50761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F2D7FCA1-D9DB-43F3-ACEF-0B3E5FA50761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83895899-E4ED-4E90-A42B-F6823F993CBC}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{48001077-B0FA-43D7-8863-EF925434C9DF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="15450" xr2:uid="{48001077-B0FA-43D7-8863-EF925434C9DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,17 +305,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF111111"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -440,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -517,10 +520,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -536,9 +542,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -576,7 +582,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -682,7 +688,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -824,7 +830,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -834,9 +840,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A5DD04-EA05-47E6-B111-91DD7D53ABF0}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="106" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.85546875" customWidth="1"/>
     <col min="2" max="2" width="64.7109375" customWidth="1"/>
@@ -848,7 +856,7 @@
     <col min="9" max="9" width="50.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.9">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -875,7 +883,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="81.599999999999994" customHeight="1">
+    <row r="2" spans="1:10" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -904,7 +912,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:10" ht="142.15" customHeight="1">
+    <row r="3" spans="1:10" ht="142.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
@@ -933,7 +941,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="10"/>
     </row>
-    <row r="4" spans="1:10" ht="86.45">
+    <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
@@ -962,7 +970,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="10"/>
     </row>
-    <row r="5" spans="1:10" ht="75" customHeight="1">
+    <row r="5" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>22</v>
       </c>
@@ -991,11 +999,11 @@
       <c r="I5" s="6"/>
       <c r="J5" s="10"/>
     </row>
-    <row r="6" spans="1:10" ht="95.45" customHeight="1">
+    <row r="6" spans="1:10" ht="95.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="26" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -1020,7 +1028,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="10"/>
     </row>
-    <row r="7" spans="1:10" ht="86.45" customHeight="1">
+    <row r="7" spans="1:10" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -1049,7 +1057,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="10"/>
     </row>
-    <row r="8" spans="1:10" ht="72">
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>36</v>
       </c>
@@ -1078,7 +1086,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="10"/>
     </row>
-    <row r="9" spans="1:10" ht="72">
+    <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>42</v>
       </c>
@@ -1107,7 +1115,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:10" ht="28.9">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>48</v>
       </c>
@@ -1136,7 +1144,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:10" ht="57.6">
+    <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>54</v>
       </c>
@@ -1165,7 +1173,7 @@
       <c r="I11" s="8"/>
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:10" ht="100.9">
+    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>56</v>
       </c>
@@ -1193,7 +1201,7 @@
       </c>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
@@ -1205,7 +1213,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G14" s="13" t="s">
         <v>62</v>
       </c>

</xml_diff>